<commit_message>
Java tutorial package and selenium package added
</commit_message>
<xml_diff>
--- a/FrameWork_Selenium/DataDriven_Project/src/testData/TestData.xlsx
+++ b/FrameWork_Selenium/DataDriven_Project/src/testData/TestData.xlsx
@@ -33,13 +33,13 @@
     <t>Apache_POI_TC</t>
   </si>
   <si>
-    <t>manoj</t>
-  </si>
-  <si>
-    <t>madan123$</t>
-  </si>
-  <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>fhsfh</t>
+  </si>
+  <si>
+    <t>asfahs</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,13 +457,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>